<commit_message>
added mentor checkbox funcitonality
</commit_message>
<xml_diff>
--- a/MIT_SOLVE_Confirmed_Matches.xlsx
+++ b/MIT_SOLVE_Confirmed_Matches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryandonlan/Desktop/Colaberry/Plotly Dash Heroku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{230CA1BF-53D0-0E4D-97FA-17C5E8241B0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{55FAF0FF-F9DD-6646-9318-440C3EA6A427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{6B3F6AC7-AC55-004C-9D4D-2767788C23E4}"/>
+    <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{6B3F6AC7-AC55-004C-9D4D-2767788C23E4}"/>
   </bookViews>
   <sheets>
     <sheet name="MIT_SOLVE_Confirmed_Matches" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>MENTOR</t>
   </si>
@@ -41,7 +41,13 @@
     <t>COMMENTS</t>
   </si>
   <si>
+    <t>Elpis Solar</t>
+  </si>
+  <si>
     <t>SOLVER</t>
+  </si>
+  <si>
+    <t>Henkel</t>
   </si>
 </sst>
 </file>
@@ -393,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108CC873-A10D-4D46-916E-E586E32E4C62}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B4"/>
@@ -411,10 +417,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing matches excel sheet
</commit_message>
<xml_diff>
--- a/MIT_SOLVE_Confirmed_Matches.xlsx
+++ b/MIT_SOLVE_Confirmed_Matches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryandonlan/Desktop/Colaberry/Plotly Dash Heroku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{55FAF0FF-F9DD-6646-9318-440C3EA6A427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D939A6B-B464-FC49-906C-A59F12729E17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{6B3F6AC7-AC55-004C-9D4D-2767788C23E4}"/>
+    <workbookView xWindow="4060" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{6B3F6AC7-AC55-004C-9D4D-2767788C23E4}"/>
   </bookViews>
   <sheets>
     <sheet name="MIT_SOLVE_Confirmed_Matches" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>MENTOR</t>
   </si>
@@ -41,10 +41,22 @@
     <t>COMMENTS</t>
   </si>
   <si>
+    <t>SOLVER</t>
+  </si>
+  <si>
+    <t>MIT Environmental Solutions Initative (John Fernandez)</t>
+  </si>
+  <si>
     <t>Elpis Solar</t>
   </si>
   <si>
-    <t>SOLVER</t>
+    <t>LLamasoft</t>
+  </si>
+  <si>
+    <t>Capital One</t>
+  </si>
+  <si>
+    <t>Dost Education</t>
   </si>
   <si>
     <t>Henkel</t>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108CC873-A10D-4D46-916E-E586E32E4C62}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,7 +429,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -425,10 +437,34 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing a version that works onto git
</commit_message>
<xml_diff>
--- a/MIT_SOLVE_Confirmed_Matches.xlsx
+++ b/MIT_SOLVE_Confirmed_Matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryandonlan/Desktop/Colaberry/Plotly Dash Heroku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F3EC3F-687A-BD4C-8A7B-5CB410A002E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5274D2F0-2BE4-BA43-B005-5DD5E3BE1D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{A9E2EC56-D121-B548-806B-5CB352888F27}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>COMMENTS</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>SOLVER</t>
+  </si>
+  <si>
+    <t>Capital One</t>
   </si>
   <si>
     <t>AIR-INK: Air-Pollution to ink</t>
@@ -408,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405FC69E-0A82-5044-B0E6-FD8BA3E9E6F6}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -434,26 +437,34 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getting away from xlwings
</commit_message>
<xml_diff>
--- a/MIT_SOLVE_Confirmed_Matches.xlsx
+++ b/MIT_SOLVE_Confirmed_Matches.xlsx
@@ -1,83 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryandonlan/Desktop/Colaberry/Plotly Dash Heroku/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5274D2F0-2BE4-BA43-B005-5DD5E3BE1D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{A9E2EC56-D121-B548-806B-5CB352888F27}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17440" windowWidth="28040" xWindow="2780" yWindow="1560"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>COMMENTS</t>
-  </si>
-  <si>
-    <t>MENTOR</t>
-  </si>
-  <si>
-    <t>SOLVER</t>
-  </si>
-  <si>
-    <t>Capital One</t>
-  </si>
-  <si>
-    <t>AIR-INK: Air-Pollution to ink</t>
-  </si>
-  <si>
-    <t>MIT Environmental Solutions Initative (John Fernandez)</t>
-  </si>
-  <si>
-    <t>Putnam Associates</t>
-  </si>
-  <si>
-    <t>LLamasoft</t>
-  </si>
-  <si>
-    <t>BioCellection</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,24 +43,83 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -410,64 +419,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405FC69E-0A82-5044-B0E6-FD8BA3E9E6F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="37.6640625"/>
+    <col customWidth="1" max="2" min="2" width="43.1640625"/>
+    <col customWidth="1" max="3" min="3" width="31.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>MENTOR</t>
+        </is>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>SOLVER</t>
+        </is>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>COMMENTS</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working version to git
</commit_message>
<xml_diff>
--- a/MIT_SOLVE_Confirmed_Matches.xlsx
+++ b/MIT_SOLVE_Confirmed_Matches.xlsx
@@ -424,10 +424,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -454,17 +454,9 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>